<commit_message>
ccru - templates update: PROS-5125.
</commit_message>
<xml_diff>
--- a/Projects/CCRU/Data/Convenience Small PoS 2018.xlsx
+++ b/Projects/CCRU/Data/Convenience Small PoS 2018.xlsx
@@ -40,6 +40,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Convenience Small'!$A$1:$AO$162</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Convenience Small'!$A$1:$AO$162</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Convenience Small'!$A$1:$AO$162</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Convenience Small'!$A$1:$AO$162</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -1460,7 +1461,7 @@
     <t xml:space="preserve">Промо дисплеи: Фейсинги</t>
   </si>
   <si>
-    <t xml:space="preserve">check_number_of_scenes_with_facings_target</t>
+    <t xml:space="preserve">number of scenes with have at least target amount of facings</t>
   </si>
   <si>
     <t xml:space="preserve">COUNT</t>
@@ -2251,7 +2252,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2415,25 +2416,25 @@
   </sheetPr>
   <dimension ref="A1:AO162"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="U1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A125" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="U1" activeCellId="0" sqref="U1"/>
-      <selection pane="bottomLeft" activeCell="AC126" activeCellId="0" sqref="AC126:AF126"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A143" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="K145" activeCellId="0" sqref="K145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="9.06072874493927"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="30.1133603238866"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="9.06072874493927"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="9.18218623481781"/>
-    <col collapsed="false" hidden="false" max="10" min="9" style="0" width="9.06072874493927"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="9.78947368421053"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="2" width="21.914979757085"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="21.1821862348178"/>
-    <col collapsed="false" hidden="false" max="21" min="14" style="0" width="9.06072874493927"/>
-    <col collapsed="false" hidden="false" max="23" min="22" style="0" width="14.8097165991903"/>
-    <col collapsed="false" hidden="false" max="1025" min="24" style="0" width="9.06072874493927"/>
+    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="9.18218623481781"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="30.8502024291498"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="9.18218623481781"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="9.30364372469636"/>
+    <col collapsed="false" hidden="false" max="10" min="9" style="0" width="9.18218623481781"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="9.91093117408907"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="2" width="22.4008097165992"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="21.5465587044534"/>
+    <col collapsed="false" hidden="false" max="21" min="14" style="0" width="9.18218623481781"/>
+    <col collapsed="false" hidden="false" max="23" min="22" style="0" width="15.0526315789474"/>
+    <col collapsed="false" hidden="false" max="1025" min="24" style="0" width="9.18218623481781"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="89.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14585,7 +14586,7 @@
       </c>
       <c r="AO144" s="12"/>
     </row>
-    <row r="145" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="145" customFormat="false" ht="92.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="25" t="n">
         <v>144</v>
       </c>
@@ -14611,11 +14612,9 @@
         <v>436</v>
       </c>
       <c r="I145" s="51" t="n">
-        <v>1</v>
-      </c>
-      <c r="J145" s="51" t="n">
         <v>8</v>
       </c>
+      <c r="J145" s="51"/>
       <c r="K145" s="51"/>
       <c r="L145" s="51" t="s">
         <v>206</v>
@@ -14670,7 +14669,7 @@
       </c>
       <c r="AO145" s="12"/>
     </row>
-    <row r="146" customFormat="false" ht="65.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="146" customFormat="false" ht="56.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="15" t="n">
         <v>145</v>
       </c>
@@ -15872,12 +15871,12 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="AC126:AF126 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.06072874493927"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.18218623481781"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15909,12 +15908,12 @@
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="AC126:AF126 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.06072874493927"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.18218623481781"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>